<commit_message>
Bug fixes with color and the stupid Levels
</commit_message>
<xml_diff>
--- a/Colors/color_themes.xlsx
+++ b/Colors/color_themes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\brickr\brickr\Colors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4FEEEC-B56C-4E49-8C51-B2F9AE93005D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDCD84-BA34-4166-877C-4DB669A9AFA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1740" windowWidth="13200" windowHeight="11970" xr2:uid="{74401F24-5269-4584-838A-1B6CD1B3EC6C}"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="8190" windowHeight="11970" xr2:uid="{74401F24-5269-4584-838A-1B6CD1B3EC6C}"/>
   </bookViews>
   <sheets>
     <sheet name="theme colors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>brickrID</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>blue</t>
+  </si>
+  <si>
+    <t>elves</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1406,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A86493-8124-4CB2-A63E-532771C85E80}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AI42"/>
+  <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -1416,28 +1419,28 @@
     <col min="3" max="3" width="3.6328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="3.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="4.08984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.26953125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="4.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.90625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="2.6328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.36328125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="4.54296875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.26953125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="4.54296875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="2.6328125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.1796875" style="2" customWidth="1"/>
-    <col min="18" max="19" width="2.6328125" style="2" customWidth="1"/>
-    <col min="20" max="21" width="4.26953125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="4.453125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="20.6328125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="10.54296875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="29" width="8.7265625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="16384" width="8.7265625" style="2"/>
+    <col min="6" max="7" width="3.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.90625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.36328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.6328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3.54296875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="4.36328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.54296875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.26953125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.54296875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="2.6328125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.1796875" style="2" customWidth="1"/>
+    <col min="19" max="20" width="2.6328125" style="2" customWidth="1"/>
+    <col min="21" max="22" width="4.26953125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="4.453125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="20.6328125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.54296875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="30" width="8.7265625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1457,70 +1460,73 @@
         <v>98</v>
       </c>
       <c r="G1" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="I1" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="K1" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="L1" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="M1" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="N1" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="O1" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="P1" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="Q1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="R1" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="S1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="T1" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>91</v>
       </c>
@@ -1540,34 +1546,34 @@
         <v>38</v>
       </c>
       <c r="G2" s="6">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6">
         <v>18</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1</v>
       </c>
       <c r="I2" s="6">
         <v>1</v>
       </c>
       <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
         <v>4</v>
       </c>
-      <c r="K2" s="6">
+      <c r="L2" s="6">
         <v>1</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
         <v>16</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <v>9</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2" s="6">
         <v>7</v>
       </c>
-      <c r="O2" s="6">
+      <c r="P2" s="6">
         <v>9</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1</v>
       </c>
       <c r="Q2" s="6">
         <v>1</v>
@@ -1578,20 +1584,20 @@
       <c r="S2" s="6">
         <v>1</v>
       </c>
-      <c r="V2" s="3">
+      <c r="T2" s="6">
         <v>1</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="3">
+        <v>1</v>
+      </c>
+      <c r="X2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1</v>
       </c>
       <c r="Y2" s="2">
         <v>1</v>
       </c>
       <c r="Z2" s="2">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="2">
         <v>244</v>
@@ -1599,11 +1605,14 @@
       <c r="AB2" s="2">
         <v>244</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="2">
+        <v>244</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="49" t="s">
         <v>92</v>
       </c>
@@ -1638,10 +1647,10 @@
         <v>6</v>
       </c>
       <c r="L3" s="50">
+        <v>6</v>
+      </c>
+      <c r="M3" s="50">
         <v>32</v>
-      </c>
-      <c r="M3" s="50">
-        <v>6</v>
       </c>
       <c r="N3" s="50">
         <v>6</v>
@@ -1661,33 +1670,36 @@
       <c r="S3" s="50">
         <v>6</v>
       </c>
-      <c r="V3" s="3">
-        <f>V2+1</f>
+      <c r="T3" s="50">
+        <v>6</v>
+      </c>
+      <c r="W3" s="3">
+        <f>W2+1</f>
         <v>2</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <v>2</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>5</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>204</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>185</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AC3" s="2">
         <v>141</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
@@ -1707,34 +1719,34 @@
         <v>19</v>
       </c>
       <c r="G4" s="6">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6">
         <v>5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>16</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>4</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>37</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>32</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>6</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>15</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <v>5</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="6">
         <v>4</v>
-      </c>
-      <c r="P4" s="6">
-        <v>3</v>
       </c>
       <c r="Q4" s="6">
         <v>3</v>
@@ -1743,35 +1755,38 @@
         <v>3</v>
       </c>
       <c r="S4" s="6">
+        <v>3</v>
+      </c>
+      <c r="T4" s="6">
         <v>4</v>
       </c>
-      <c r="V4" s="3">
-        <f t="shared" ref="V4:V42" si="0">V3+1</f>
+      <c r="W4" s="3">
+        <f t="shared" ref="W4:W42" si="0">W3+1</f>
         <v>3</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="X4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Y4" s="2">
         <v>3</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Z4" s="2">
         <v>21</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AA4" s="2">
         <v>180</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>0</v>
       </c>
       <c r="AB4" s="2">
         <v>0</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AC4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
@@ -1791,34 +1806,34 @@
         <v>20</v>
       </c>
       <c r="G5" s="6">
+        <v>38</v>
+      </c>
+      <c r="H5" s="6">
         <v>3</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>11</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>14</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>29</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>5</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>29</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>18</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>21</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>1</v>
-      </c>
-      <c r="P5" s="6">
-        <v>14</v>
       </c>
       <c r="Q5" s="6">
         <v>14</v>
@@ -1827,35 +1842,38 @@
         <v>14</v>
       </c>
       <c r="S5" s="6">
+        <v>14</v>
+      </c>
+      <c r="T5" s="6">
         <v>13</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="X5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <v>4</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>23</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>30</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>90</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AC5" s="2">
         <v>168</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -1875,71 +1893,74 @@
         <v>21</v>
       </c>
       <c r="G6" s="6">
+        <v>37</v>
+      </c>
+      <c r="H6" s="6">
         <v>29</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>18</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>5</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>1</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>4</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>25</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <v>40</v>
-      </c>
-      <c r="N6" s="6">
-        <v>3</v>
       </c>
       <c r="O6" s="6">
         <v>3</v>
       </c>
       <c r="P6" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="6">
         <v>5</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
         <v>29</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="6">
         <v>5</v>
       </c>
-      <c r="S6" s="6">
+      <c r="T6" s="6">
         <v>21</v>
       </c>
-      <c r="V6" s="3">
+      <c r="W6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W6" s="45" t="s">
+      <c r="X6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Y6" s="2">
         <v>5</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Z6" s="2">
         <v>24</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>250</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <v>200</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AC6" s="2">
         <v>10</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AD6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>93</v>
       </c>
@@ -1959,76 +1980,79 @@
         <v>29</v>
       </c>
       <c r="G7" s="6">
+        <v>41</v>
+      </c>
+      <c r="H7" s="6">
         <v>6</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>27</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <v>3</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <v>21</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <v>3</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <v>10</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>11</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>15</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>5</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>7</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>5</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="6">
         <v>7</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="6">
         <v>24</v>
       </c>
-      <c r="V7" s="3">
+      <c r="W7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="X7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Y7" s="2">
         <v>6</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <v>26</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>27</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <v>42</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AC7" s="2">
         <v>52</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AD7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="6">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6">
         <v>17</v>
@@ -2043,76 +2067,79 @@
         <v>39</v>
       </c>
       <c r="G8" s="6">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6">
         <v>31</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <v>17</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <v>9</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <v>31</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <v>6</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>32</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>27</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>14</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>10</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>4</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>15</v>
       </c>
-      <c r="R8" s="6">
+      <c r="S8" s="6">
         <v>4</v>
       </c>
-      <c r="S8" s="6">
+      <c r="T8" s="6">
         <v>26</v>
       </c>
-      <c r="V8" s="3">
+      <c r="W8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="W8" s="11" t="s">
+      <c r="X8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <v>7</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <v>28</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
         <v>0</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <v>133</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AC8" s="2">
         <v>43</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B9" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <v>32</v>
@@ -2127,71 +2154,74 @@
         <v>22</v>
       </c>
       <c r="G9" s="6">
+        <v>22</v>
+      </c>
+      <c r="H9" s="6">
         <v>9</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <v>2</v>
       </c>
-      <c r="I9" s="6">
+      <c r="J9" s="6">
         <v>36</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <v>39</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <v>19</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <v>5</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <v>3</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <v>4</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <v>6</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>32</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>7</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>32</v>
       </c>
-      <c r="S9" s="6">
+      <c r="T9" s="6">
         <v>30</v>
       </c>
-      <c r="V9" s="3">
+      <c r="W9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="W9" s="46" t="s">
+      <c r="X9" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <v>8</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>192</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>95</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <v>49</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <v>9</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AD9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>93</v>
       </c>
@@ -2211,59 +2241,59 @@
         <v>41</v>
       </c>
       <c r="G10" s="6">
+        <v>24</v>
+      </c>
+      <c r="H10" s="6">
         <v>17</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>4</v>
       </c>
-      <c r="I10" s="6">
+      <c r="J10" s="6">
         <v>7</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <v>36</v>
       </c>
-      <c r="K10" s="6">
+      <c r="L10" s="6">
         <v>29</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <v>19</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="6">
         <v>17</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <v>20</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <v>16</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>38</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>24</v>
       </c>
-      <c r="R10" s="6">
+      <c r="S10" s="6">
         <v>38</v>
       </c>
-      <c r="S10" s="6">
+      <c r="T10" s="6">
         <v>36</v>
       </c>
-      <c r="V10" s="3">
+      <c r="W10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="W10" s="12" t="s">
+      <c r="X10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Y10" s="2">
         <v>9</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <v>194</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>150</v>
       </c>
       <c r="AA10" s="2">
         <v>150</v>
@@ -2271,16 +2301,19 @@
       <c r="AB10" s="2">
         <v>150</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AC10" s="2">
+        <v>150</v>
+      </c>
+      <c r="AD10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B11" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6">
         <v>24</v>
@@ -2295,57 +2328,57 @@
         <v>24</v>
       </c>
       <c r="G11" s="6">
+        <v>21</v>
+      </c>
+      <c r="H11" s="6">
         <v>10</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>35</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <v>18</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <v>33</v>
       </c>
-      <c r="K11" s="6">
+      <c r="L11" s="6">
         <v>24</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="6">
         <v>18</v>
       </c>
-      <c r="M11" s="6">
+      <c r="N11" s="6">
         <v>39</v>
       </c>
-      <c r="N11" s="6">
+      <c r="O11" s="6">
         <v>1</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <v>17</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6">
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
         <v>21</v>
       </c>
-      <c r="R11" s="6">
-        <v>18</v>
-      </c>
       <c r="S11" s="6">
+        <v>19</v>
+      </c>
+      <c r="T11" s="6">
         <v>37</v>
       </c>
-      <c r="V11" s="3">
+      <c r="W11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="X11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Y11" s="2">
         <v>10</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <v>199</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>100</v>
       </c>
       <c r="AA11" s="2">
         <v>100</v>
@@ -2353,11 +2386,14 @@
       <c r="AB11" s="2">
         <v>100</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AC11" s="2">
+        <v>100</v>
+      </c>
+      <c r="AD11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>93</v>
       </c>
@@ -2377,67 +2413,70 @@
         <v>25</v>
       </c>
       <c r="G12" s="6">
+        <v>17</v>
+      </c>
+      <c r="H12" s="6">
         <v>32</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <v>41</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <v>10</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <v>41</v>
       </c>
-      <c r="K12" s="6">
+      <c r="L12" s="6">
         <v>25</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <v>31</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N12" s="6">
         <v>35</v>
-      </c>
-      <c r="N12" s="6">
-        <v>29</v>
       </c>
       <c r="O12" s="6">
         <v>29</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6">
+      <c r="P12" s="6">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6">
         <v>4</v>
       </c>
-      <c r="R12" s="6">
+      <c r="S12" s="6">
         <v>29</v>
       </c>
-      <c r="S12" s="6"/>
-      <c r="V12" s="3">
+      <c r="T12" s="6"/>
+      <c r="W12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="W12" s="14" t="s">
+      <c r="X12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="X12" s="2">
+      <c r="Y12" s="2">
         <v>11</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Z12" s="2">
         <v>18</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AA12" s="2">
         <v>187</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>128</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AC12" s="2">
         <v>90</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AD12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>93</v>
       </c>
@@ -2457,67 +2496,70 @@
         <v>31</v>
       </c>
       <c r="G13" s="6">
+        <v>32</v>
+      </c>
+      <c r="H13" s="6">
         <v>2</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <v>40</v>
       </c>
-      <c r="I13" s="6">
+      <c r="J13" s="6">
         <v>21</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <v>30</v>
       </c>
-      <c r="K13" s="6">
+      <c r="L13" s="6">
         <v>39</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <v>24</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="6">
         <v>31</v>
       </c>
-      <c r="N13" s="6">
+      <c r="O13" s="6">
         <v>32</v>
       </c>
-      <c r="O13" s="6">
+      <c r="P13" s="6">
         <v>19</v>
       </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6">
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6">
         <v>32</v>
       </c>
-      <c r="R13" s="6">
+      <c r="S13" s="6">
         <v>15</v>
       </c>
-      <c r="S13" s="6"/>
-      <c r="V13" s="3">
+      <c r="T13" s="6"/>
+      <c r="W13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="W13" s="15" t="s">
+      <c r="X13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Y13" s="2">
         <v>12</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Z13" s="2">
         <v>37</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AA13" s="2">
         <v>88</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AB13" s="2">
         <v>171</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AC13" s="2">
         <v>65</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AD13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>93</v>
       </c>
@@ -2537,67 +2579,70 @@
         <v>30</v>
       </c>
       <c r="G14" s="6">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6">
         <v>14</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>26</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <v>29</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <v>35</v>
       </c>
-      <c r="K14" s="6">
+      <c r="L14" s="6">
         <v>41</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <v>38</v>
       </c>
-      <c r="M14" s="6">
+      <c r="N14" s="6">
         <v>7</v>
       </c>
-      <c r="N14" s="6">
+      <c r="O14" s="6">
         <v>19</v>
       </c>
-      <c r="O14" s="6">
+      <c r="P14" s="6">
         <v>18</v>
       </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6">
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6">
         <v>25</v>
       </c>
-      <c r="R14" s="6">
+      <c r="S14" s="6">
         <v>24</v>
       </c>
-      <c r="S14" s="6"/>
-      <c r="V14" s="3">
+      <c r="T14" s="6"/>
+      <c r="W14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="W14" s="16" t="s">
+      <c r="X14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="X14" s="2">
+      <c r="Y14" s="2">
         <v>13</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Z14" s="2">
         <v>102</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AA14" s="2">
         <v>115</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AB14" s="2">
         <v>150</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AC14" s="2">
         <v>200</v>
       </c>
-      <c r="AC14" s="2" t="s">
+      <c r="AD14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>93</v>
       </c>
@@ -2617,67 +2662,70 @@
         <v>15</v>
       </c>
       <c r="G15" s="6">
+        <v>18</v>
+      </c>
+      <c r="H15" s="6">
         <v>41</v>
-      </c>
-      <c r="H15" s="6">
-        <v>39</v>
       </c>
       <c r="I15" s="6">
         <v>39</v>
       </c>
       <c r="J15" s="6">
+        <v>39</v>
+      </c>
+      <c r="K15" s="6">
         <v>24</v>
-      </c>
-      <c r="K15" s="6">
-        <v>36</v>
       </c>
       <c r="L15" s="6">
         <v>36</v>
       </c>
       <c r="M15" s="6">
+        <v>36</v>
+      </c>
+      <c r="N15" s="6">
         <v>12</v>
       </c>
-      <c r="N15" s="6">
+      <c r="O15" s="6">
         <v>39</v>
       </c>
-      <c r="O15" s="6">
+      <c r="P15" s="6">
         <v>2</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6">
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6">
         <v>19</v>
       </c>
-      <c r="R15" s="6">
+      <c r="S15" s="6">
         <v>21</v>
       </c>
-      <c r="S15" s="6"/>
-      <c r="V15" s="3">
+      <c r="T15" s="6"/>
+      <c r="W15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="W15" s="17" t="s">
+      <c r="X15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="X15" s="2">
+      <c r="Y15" s="2">
         <v>14</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Z15" s="2">
         <v>106</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AA15" s="2">
         <v>214</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AB15" s="2">
         <v>121</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AC15" s="2">
         <v>35</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AD15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
@@ -2694,68 +2742,69 @@
       <c r="F16" s="6">
         <v>14</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6">
         <v>16</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <v>31</v>
       </c>
-      <c r="I16" s="6">
+      <c r="J16" s="6">
         <v>6</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <v>26</v>
       </c>
-      <c r="K16" s="6">
+      <c r="L16" s="6">
         <v>21</v>
       </c>
-      <c r="L16" s="6">
+      <c r="M16" s="6">
         <v>17</v>
       </c>
-      <c r="M16" s="6">
+      <c r="N16" s="6">
         <v>28</v>
       </c>
-      <c r="N16" s="6">
+      <c r="O16" s="6">
         <v>41</v>
       </c>
-      <c r="O16" s="6">
+      <c r="P16" s="6">
         <v>30</v>
       </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6">
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6">
         <v>20</v>
       </c>
-      <c r="R16" s="6">
+      <c r="S16" s="6">
         <v>25</v>
       </c>
-      <c r="S16" s="6"/>
-      <c r="V16" s="3">
+      <c r="T16" s="6"/>
+      <c r="W16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="W16" s="18" t="s">
+      <c r="X16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="X16" s="2">
+      <c r="Y16" s="2">
         <v>15</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="2">
         <v>119</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AA16" s="2">
         <v>165</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AB16" s="2">
         <v>202</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AC16" s="2">
         <v>24</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AD16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>93</v>
       </c>
@@ -2768,54 +2817,55 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="6">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
         <v>13</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <v>28</v>
       </c>
-      <c r="K17" s="6">
+      <c r="L17" s="6">
         <v>20</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="6">
         <v>40</v>
       </c>
-      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
-      <c r="R17" s="6">
+      <c r="R17" s="6"/>
+      <c r="S17" s="6">
         <v>20</v>
       </c>
-      <c r="S17" s="6"/>
-      <c r="V17" s="3">
+      <c r="T17" s="6"/>
+      <c r="W17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="W17" s="42" t="s">
+      <c r="X17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Y17" s="2">
         <v>16</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Z17" s="2">
         <v>140</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AA17" s="2">
         <v>25</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AB17" s="2">
         <v>50</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="AC17" s="2">
         <v>90</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AD17" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>93</v>
       </c>
@@ -2838,34 +2888,37 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="V18" s="3">
+      <c r="S18" s="6">
+        <v>18</v>
+      </c>
+      <c r="T18" s="6"/>
+      <c r="W18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="W18" s="43" t="s">
+      <c r="X18" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="X18" s="2">
+      <c r="Y18" s="2">
         <v>17</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Z18" s="2">
         <v>141</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="AA18" s="2">
         <v>0</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AB18" s="2">
         <v>69</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="AC18" s="2">
         <v>26</v>
       </c>
-      <c r="AC18" s="2" t="s">
+      <c r="AD18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>93</v>
       </c>
@@ -2889,33 +2942,34 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
-      <c r="V19" s="3">
+      <c r="T19" s="6"/>
+      <c r="W19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W19" s="44" t="s">
+      <c r="X19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="X19" s="2">
+      <c r="Y19" s="2">
         <v>18</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Z19" s="2">
         <v>154</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AA19" s="2">
         <v>114</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AB19" s="2">
         <v>0</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="AC19" s="2">
         <v>18</v>
       </c>
-      <c r="AC19" s="2" t="s">
+      <c r="AD19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
@@ -2939,33 +2993,34 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="V20" s="3">
+      <c r="T20" s="6"/>
+      <c r="W20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="W20" s="19" t="s">
+      <c r="X20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="X20" s="2">
+      <c r="Y20" s="2">
         <v>19</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Z20" s="2">
         <v>221</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AA20" s="2">
         <v>200</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AB20" s="2">
         <v>80</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AC20" s="2">
         <v>155</v>
       </c>
-      <c r="AC20" s="2" t="s">
+      <c r="AD20" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>93</v>
       </c>
@@ -2989,33 +3044,34 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
-      <c r="V21" s="3">
+      <c r="T21" s="6"/>
+      <c r="W21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="W21" s="20" t="s">
+      <c r="X21" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="X21" s="2">
+      <c r="Y21" s="2">
         <v>20</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Z21" s="2">
         <v>222</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AA21" s="2">
         <v>255</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AB21" s="2">
         <v>158</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="AC21" s="2">
         <v>205</v>
       </c>
-      <c r="AC21" s="2" t="s">
+      <c r="AD21" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>93</v>
       </c>
@@ -3039,33 +3095,34 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
-      <c r="V22" s="3">
+      <c r="T22" s="6"/>
+      <c r="W22" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="W22" s="21" t="s">
+      <c r="X22" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="X22" s="2">
+      <c r="Y22" s="2">
         <v>21</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="Z22" s="2">
         <v>322</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="AA22" s="2">
         <v>104</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="AB22" s="2">
         <v>195</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="AC22" s="2">
         <v>226</v>
       </c>
-      <c r="AC22" s="2" t="s">
+      <c r="AD22" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>93</v>
       </c>
@@ -3089,33 +3146,34 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
-      <c r="V23" s="3">
+      <c r="T23" s="6"/>
+      <c r="W23" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="W23" s="22" t="s">
+      <c r="X23" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Y23" s="2">
         <v>22</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Z23" s="2">
         <v>324</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AA23" s="2">
         <v>154</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AB23" s="2">
         <v>118</v>
       </c>
-      <c r="AB23" s="2">
+      <c r="AC23" s="2">
         <v>174</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AD23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
@@ -3139,33 +3197,34 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
-      <c r="V24" s="3">
+      <c r="T24" s="6"/>
+      <c r="W24" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="W24" s="23" t="s">
+      <c r="X24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="X24" s="2">
+      <c r="Y24" s="2">
         <v>23</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Z24" s="2">
         <v>38</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="AA24" s="2">
         <v>145</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="AB24" s="2">
         <v>80</v>
       </c>
-      <c r="AB24" s="2">
+      <c r="AC24" s="2">
         <v>28</v>
       </c>
-      <c r="AC24" s="2" t="s">
+      <c r="AD24" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
@@ -3189,493 +3248,494 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
-      <c r="V25" s="3">
+      <c r="T25" s="6"/>
+      <c r="W25" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="W25" s="24" t="s">
+      <c r="X25" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="X25" s="2">
+      <c r="Y25" s="2">
         <v>24</v>
       </c>
-      <c r="Y25" s="2">
+      <c r="Z25" s="2">
         <v>107</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AA25" s="2">
         <v>0</v>
       </c>
-      <c r="AA25" s="2">
+      <c r="AB25" s="2">
         <v>152</v>
       </c>
-      <c r="AB25" s="2">
+      <c r="AC25" s="2">
         <v>148</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AD25" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V26" s="3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W26" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="W26" s="25" t="s">
+      <c r="X26" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="X26" s="2">
+      <c r="Y26" s="2">
         <v>25</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="Z26" s="2">
         <v>124</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="AA26" s="2">
         <v>144</v>
       </c>
-      <c r="AA26" s="2">
+      <c r="AB26" s="2">
         <v>31</v>
       </c>
-      <c r="AB26" s="2">
+      <c r="AC26" s="2">
         <v>118</v>
       </c>
-      <c r="AC26" s="2" t="s">
+      <c r="AD26" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V27" s="3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W27" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="W27" s="26" t="s">
+      <c r="X27" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="X27" s="2">
+      <c r="Y27" s="2">
         <v>26</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="Z27" s="2">
         <v>135</v>
       </c>
-      <c r="Z27" s="2">
+      <c r="AA27" s="2">
         <v>112</v>
       </c>
-      <c r="AA27" s="2">
+      <c r="AB27" s="2">
         <v>129</v>
       </c>
-      <c r="AB27" s="2">
+      <c r="AC27" s="2">
         <v>154</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AD27" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V28" s="3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W28" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="W28" s="27" t="s">
+      <c r="X28" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="X28" s="2">
+      <c r="Y28" s="2">
         <v>27</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="Z28" s="2">
         <v>138</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="AA28" s="2">
         <v>137</v>
       </c>
-      <c r="AA28" s="2">
+      <c r="AB28" s="2">
         <v>125</v>
       </c>
-      <c r="AB28" s="2">
+      <c r="AC28" s="2">
         <v>98</v>
       </c>
-      <c r="AC28" s="2" t="s">
+      <c r="AD28" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V29" s="3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W29" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="W29" s="28" t="s">
+      <c r="X29" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="X29" s="2">
+      <c r="Y29" s="2">
         <v>28</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="Z29" s="2">
         <v>151</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="AA29" s="2">
         <v>112</v>
       </c>
-      <c r="AA29" s="2">
+      <c r="AB29" s="2">
         <v>142</v>
       </c>
-      <c r="AB29" s="2">
+      <c r="AC29" s="2">
         <v>124</v>
       </c>
-      <c r="AC29" s="2" t="s">
+      <c r="AD29" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V30" s="3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W30" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="W30" s="29" t="s">
+      <c r="X30" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="X30" s="2">
+      <c r="Y30" s="2">
         <v>29</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="Z30" s="2">
         <v>191</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="AA30" s="2">
         <v>252</v>
       </c>
-      <c r="AA30" s="2">
+      <c r="AB30" s="2">
         <v>172</v>
       </c>
-      <c r="AB30" s="2">
+      <c r="AC30" s="2">
         <v>0</v>
       </c>
-      <c r="AC30" s="2" t="s">
+      <c r="AD30" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V31" s="3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W31" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="W31" s="30" t="s">
+      <c r="X31" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="X31" s="2">
+      <c r="Y31" s="2">
         <v>30</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="Z31" s="2">
         <v>212</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="AA31" s="2">
         <v>157</v>
       </c>
-      <c r="AA31" s="2">
+      <c r="AB31" s="2">
         <v>195</v>
       </c>
-      <c r="AB31" s="2">
+      <c r="AC31" s="2">
         <v>247</v>
       </c>
-      <c r="AC31" s="2" t="s">
+      <c r="AD31" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="V32" s="3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="W32" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="W32" s="31" t="s">
+      <c r="X32" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="X32" s="2">
+      <c r="Y32" s="2">
         <v>31</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="Z32" s="2">
         <v>226</v>
       </c>
-      <c r="Z32" s="2">
+      <c r="AA32" s="2">
         <v>255</v>
       </c>
-      <c r="AA32" s="2">
+      <c r="AB32" s="2">
         <v>236</v>
       </c>
-      <c r="AB32" s="2">
+      <c r="AC32" s="2">
         <v>108</v>
       </c>
-      <c r="AC32" s="2" t="s">
+      <c r="AD32" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V33" s="3">
+    <row r="33" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W33" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="W33" s="41" t="s">
+      <c r="X33" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="X33" s="2">
+      <c r="Y33" s="2">
         <v>32</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="Z33" s="2">
         <v>268</v>
       </c>
-      <c r="Z33" s="2">
+      <c r="AA33" s="2">
         <v>68</v>
       </c>
-      <c r="AA33" s="2">
+      <c r="AB33" s="2">
         <v>26</v>
       </c>
-      <c r="AB33" s="2">
+      <c r="AC33" s="2">
         <v>145</v>
       </c>
-      <c r="AC33" s="2" t="s">
+      <c r="AD33" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V34" s="3">
+    <row r="34" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W34" s="3">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="W34" s="32" t="s">
+      <c r="X34" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="X34" s="2">
+      <c r="Y34" s="2">
         <v>33</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="Z34" s="2">
         <v>283</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="AA34" s="2">
         <v>225</v>
       </c>
-      <c r="AA34" s="2">
+      <c r="AB34" s="2">
         <v>190</v>
       </c>
-      <c r="AB34" s="2">
+      <c r="AC34" s="2">
         <v>161</v>
       </c>
-      <c r="AC34" s="2" t="s">
+      <c r="AD34" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V35" s="3">
+    <row r="35" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W35" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="W35" s="33" t="s">
+      <c r="X35" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="X35" s="2">
+      <c r="Y35" s="2">
         <v>34</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="Z35" s="2">
         <v>308</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="AA35" s="2">
         <v>53</v>
       </c>
-      <c r="AA35" s="2">
+      <c r="AB35" s="2">
         <v>33</v>
       </c>
-      <c r="AB35" s="2">
+      <c r="AC35" s="2">
         <v>0</v>
       </c>
-      <c r="AC35" s="2" t="s">
+      <c r="AD35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V36" s="3">
+    <row r="36" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W36" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="W36" s="34" t="s">
+      <c r="X36" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="X36" s="2">
+      <c r="Y36" s="2">
         <v>35</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="Z36" s="2">
         <v>312</v>
       </c>
-      <c r="Z36" s="2">
+      <c r="AA36" s="2">
         <v>170</v>
       </c>
-      <c r="AA36" s="2">
+      <c r="AB36" s="2">
         <v>125</v>
       </c>
-      <c r="AB36" s="2">
+      <c r="AC36" s="2">
         <v>85</v>
       </c>
-      <c r="AC36" s="2" t="s">
+      <c r="AD36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V37" s="3">
+    <row r="37" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W37" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="W37" s="37" t="s">
+      <c r="X37" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="X37" s="2">
+      <c r="Y37" s="2">
         <v>36</v>
       </c>
-      <c r="Y37" s="2">
+      <c r="Z37" s="2">
         <v>321</v>
       </c>
-      <c r="Z37" s="2">
+      <c r="AA37" s="2">
         <v>70</v>
       </c>
-      <c r="AA37" s="2">
+      <c r="AB37" s="2">
         <v>155</v>
       </c>
-      <c r="AB37" s="2">
+      <c r="AC37" s="2">
         <v>195</v>
       </c>
-      <c r="AC37" s="2" t="s">
+      <c r="AD37" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V38" s="3">
+    <row r="38" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W38" s="3">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="W38" s="38" t="s">
+      <c r="X38" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="X38" s="2">
+      <c r="Y38" s="2">
         <v>37</v>
       </c>
-      <c r="Y38" s="2">
+      <c r="Z38" s="2">
         <v>323</v>
       </c>
-      <c r="Z38" s="2">
+      <c r="AA38" s="2">
         <v>211</v>
       </c>
-      <c r="AA38" s="2">
+      <c r="AB38" s="2">
         <v>242</v>
       </c>
-      <c r="AB38" s="2">
+      <c r="AC38" s="2">
         <v>234</v>
       </c>
-      <c r="AC38" s="2" t="s">
+      <c r="AD38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V39" s="3">
+    <row r="39" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W39" s="3">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="W39" s="39" t="s">
+      <c r="X39" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="X39" s="2">
+      <c r="Y39" s="2">
         <v>38</v>
       </c>
-      <c r="Y39" s="2">
+      <c r="Z39" s="2">
         <v>325</v>
       </c>
-      <c r="Z39" s="2">
+      <c r="AA39" s="2">
         <v>205</v>
       </c>
-      <c r="AA39" s="2">
+      <c r="AB39" s="2">
         <v>164</v>
       </c>
-      <c r="AB39" s="2">
+      <c r="AC39" s="2">
         <v>222</v>
       </c>
-      <c r="AC39" s="2" t="s">
+      <c r="AD39" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V40" s="3">
+    <row r="40" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W40" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="W40" s="40" t="s">
+      <c r="X40" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="X40" s="2">
+      <c r="Y40" s="2">
         <v>39</v>
       </c>
-      <c r="Y40" s="2">
+      <c r="Z40" s="2">
         <v>326</v>
       </c>
-      <c r="Z40" s="2">
+      <c r="AA40" s="2">
         <v>226</v>
       </c>
-      <c r="AA40" s="2">
+      <c r="AB40" s="2">
         <v>249</v>
       </c>
-      <c r="AB40" s="2">
+      <c r="AC40" s="2">
         <v>154</v>
       </c>
-      <c r="AC40" s="2" t="s">
+      <c r="AD40" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V41" s="3">
+    <row r="41" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W41" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="W41" s="35" t="s">
+      <c r="X41" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="X41" s="2">
+      <c r="Y41" s="2">
         <v>40</v>
       </c>
-      <c r="Y41" s="2">
+      <c r="Z41" s="2">
         <v>330</v>
       </c>
-      <c r="Z41" s="2">
+      <c r="AA41" s="2">
         <v>139</v>
       </c>
-      <c r="AA41" s="2">
+      <c r="AB41" s="2">
         <v>132</v>
       </c>
-      <c r="AB41" s="2">
+      <c r="AC41" s="2">
         <v>79</v>
       </c>
-      <c r="AC41" s="2" t="s">
+      <c r="AD41" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="22:29" x14ac:dyDescent="0.35">
-      <c r="V42" s="3">
+    <row r="42" spans="23:30" x14ac:dyDescent="0.35">
+      <c r="W42" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="W42" s="36" t="s">
+      <c r="X42" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="X42" s="2">
+      <c r="Y42" s="2">
         <v>41</v>
       </c>
-      <c r="Y42" s="2">
+      <c r="Z42" s="2">
         <v>353</v>
       </c>
-      <c r="Z42" s="2">
+      <c r="AA42" s="2">
         <v>240</v>
       </c>
-      <c r="AA42" s="2">
+      <c r="AB42" s="2">
         <v>109</v>
       </c>
-      <c r="AB42" s="2">
+      <c r="AC42" s="2">
         <v>120</v>
       </c>
-      <c r="AC42" s="2" t="s">
+      <c r="AD42" s="2" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:S25">
+  <conditionalFormatting sqref="B2:T25">
     <cfRule type="expression" dxfId="42" priority="44">
       <formula>ISBLANK(B2)</formula>
     </cfRule>
@@ -3683,127 +3743,127 @@
       <formula>"isblank(B2)"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="46" stopIfTrue="1">
-      <formula>B2=$V$2</formula>
+      <formula>B2=$W$2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="39" priority="47" stopIfTrue="1">
-      <formula>B2=$V$3</formula>
+      <formula>B2=$W$3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="38" priority="48" stopIfTrue="1">
-      <formula>B2=$V$4</formula>
+      <formula>B2=$W$4</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="49" stopIfTrue="1">
-      <formula>B2=$V$5</formula>
+      <formula>B2=$W$5</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="50" stopIfTrue="1">
-      <formula>B2=$V$6</formula>
+      <formula>B2=$W$6</formula>
     </cfRule>
     <cfRule type="expression" dxfId="35" priority="51" stopIfTrue="1">
-      <formula>B2=$V$7</formula>
+      <formula>B2=$W$7</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="52" stopIfTrue="1">
-      <formula>B2=$V$8</formula>
+      <formula>B2=$W$8</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="53" stopIfTrue="1">
-      <formula>B2=$V$9</formula>
+      <formula>B2=$W$9</formula>
     </cfRule>
     <cfRule type="expression" dxfId="32" priority="54" stopIfTrue="1">
-      <formula>B2=$V$10</formula>
+      <formula>B2=$W$10</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="55" stopIfTrue="1">
-      <formula>B2=$V$11</formula>
+      <formula>B2=$W$11</formula>
     </cfRule>
     <cfRule type="expression" dxfId="30" priority="56" stopIfTrue="1">
-      <formula>B2=$V$12</formula>
+      <formula>B2=$W$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="29" priority="57" stopIfTrue="1">
-      <formula>B2=$V$13</formula>
+      <formula>B2=$W$13</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="58" stopIfTrue="1">
-      <formula>B2=$V$14</formula>
+      <formula>B2=$W$14</formula>
     </cfRule>
     <cfRule type="expression" dxfId="27" priority="59" stopIfTrue="1">
-      <formula>B2=$V$15</formula>
+      <formula>B2=$W$15</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="60" stopIfTrue="1">
-      <formula>B2=$V$16</formula>
+      <formula>B2=$W$16</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="61" stopIfTrue="1">
-      <formula>B2=$V$17</formula>
+      <formula>B2=$W$17</formula>
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="62" stopIfTrue="1">
-      <formula>B2=$V$18</formula>
+      <formula>B2=$W$18</formula>
     </cfRule>
     <cfRule type="expression" dxfId="23" priority="63" stopIfTrue="1">
-      <formula>B2=$V$19</formula>
+      <formula>B2=$W$19</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="64" stopIfTrue="1">
-      <formula>B2=$V$20</formula>
+      <formula>B2=$W$20</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="65" stopIfTrue="1">
-      <formula>B2=$V$21</formula>
+      <formula>B2=$W$21</formula>
     </cfRule>
     <cfRule type="expression" dxfId="20" priority="66" stopIfTrue="1">
-      <formula>B2=$V$22</formula>
+      <formula>B2=$W$22</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="67" stopIfTrue="1">
-      <formula>B2=$V$23</formula>
+      <formula>B2=$W$23</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="68" stopIfTrue="1">
-      <formula>B2=$V$24</formula>
+      <formula>B2=$W$24</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="69" stopIfTrue="1">
-      <formula>B2=$V$25</formula>
+      <formula>B2=$W$25</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="70" stopIfTrue="1">
-      <formula>B2=$V$26</formula>
+      <formula>B2=$W$26</formula>
     </cfRule>
     <cfRule type="expression" dxfId="15" priority="71" stopIfTrue="1">
-      <formula>B2=$V$27</formula>
+      <formula>B2=$W$27</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="72" stopIfTrue="1">
-      <formula>B2=$V$28</formula>
+      <formula>B2=$W$28</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="73" stopIfTrue="1">
-      <formula>B2=$V$29</formula>
+      <formula>B2=$W$29</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="74" stopIfTrue="1">
-      <formula>B2=$V$30</formula>
+      <formula>B2=$W$30</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="75" stopIfTrue="1">
-      <formula>B2=$V$31</formula>
+      <formula>B2=$W$31</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="76" stopIfTrue="1">
-      <formula>B2=$V$32</formula>
+      <formula>B2=$W$32</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="77" stopIfTrue="1">
-      <formula>B2=$V$33</formula>
+      <formula>B2=$W$33</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="78" stopIfTrue="1">
-      <formula>B2=$V$34</formula>
+      <formula>B2=$W$34</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="79" stopIfTrue="1">
-      <formula>B2=$V$35</formula>
+      <formula>B2=$W$35</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="80" stopIfTrue="1">
-      <formula>B2=$V$36</formula>
+      <formula>B2=$W$36</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="81" stopIfTrue="1">
-      <formula>B2=$V$37</formula>
+      <formula>B2=$W$37</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="82" stopIfTrue="1">
-      <formula>B2=$V$38</formula>
+      <formula>B2=$W$38</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="83" stopIfTrue="1">
-      <formula>B2=$V$39</formula>
+      <formula>B2=$W$39</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="84" stopIfTrue="1">
-      <formula>B2=$V$40</formula>
+      <formula>B2=$W$40</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="85" stopIfTrue="1">
-      <formula>B2=$V$41</formula>
+      <formula>B2=$W$41</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="86" stopIfTrue="1">
-      <formula>B2=$V$42</formula>
+      <formula>B2=$W$42</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Additional fixes but not sure why collate issues on build.
</commit_message>
<xml_diff>
--- a/Colors/color_themes.xlsx
+++ b/Colors/color_themes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\brickr\brickr\Colors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usRyaTim\Onedrive - LEGO\Documents\brickr\Colors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDCD84-BA34-4166-877C-4DB669A9AFA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{90DDCD84-BA34-4166-877C-4DB669A9AFA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{479B19F9-FA93-4329-A9BD-BF347B88AC12}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="8190" windowHeight="11970" xr2:uid="{74401F24-5269-4584-838A-1B6CD1B3EC6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74401F24-5269-4584-838A-1B6CD1B3EC6C}"/>
   </bookViews>
   <sheets>
     <sheet name="theme colors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>brickrID</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>elves</t>
+  </si>
+  <si>
+    <t>ducks</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,308 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="86">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF06D78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8B844F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2F99A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDA4DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3F2EA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF469BC3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA7D55"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF352100"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1BEA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF441A91"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEC6C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9DC3F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF708E7C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF897D62"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70819A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF901F76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009894"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF91501C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9A76AE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF68C3E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9ECD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC8509B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF720012"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00451A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF19325A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5CA18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD67923"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7396C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF58AB41"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBB805A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF646464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5F3109"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00852B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1B2A34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAC80A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1E5AA8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB40000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCB98D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F4F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1406,41 +1710,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A86493-8124-4CB2-A63E-532771C85E80}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AD42"/>
+  <dimension ref="A1:AE42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="3.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.08984375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="3.26953125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="4.90625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.6328125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3.54296875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="4.36328125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.54296875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="4.26953125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.54296875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="2.6328125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.1796875" style="2" customWidth="1"/>
-    <col min="19" max="20" width="2.6328125" style="2" customWidth="1"/>
-    <col min="21" max="22" width="4.26953125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="4.453125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="20.6328125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.54296875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="30" width="8.7265625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="3.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="5.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.5546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3.21875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="4.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6" style="2" customWidth="1"/>
+    <col min="18" max="18" width="2.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="5.21875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="2.77734375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.33203125" style="2" customWidth="1"/>
+    <col min="22" max="23" width="4.21875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="10.5546875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="31" width="8.77734375" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1448,85 +1754,88 @@
         <v>94</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F1" s="47" t="s">
         <v>98</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="H1" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="K1" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" s="47" t="s">
+      <c r="P1" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" s="47" t="s">
+      <c r="R1" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="S1" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="T1" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>91</v>
       </c>
@@ -1534,49 +1843,49 @@
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="6">
         <v>38</v>
       </c>
       <c r="G2" s="6">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6">
         <v>9</v>
-      </c>
-      <c r="H2" s="6">
-        <v>18</v>
       </c>
       <c r="I2" s="6">
         <v>1</v>
       </c>
       <c r="J2" s="6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K2" s="6">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L2" s="6">
         <v>1</v>
       </c>
       <c r="M2" s="6">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="N2" s="6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="O2" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P2" s="6">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R2" s="6">
         <v>1</v>
@@ -1587,20 +1896,20 @@
       <c r="T2" s="6">
         <v>1</v>
       </c>
-      <c r="W2" s="3">
+      <c r="U2" s="6">
+        <v>16</v>
+      </c>
+      <c r="X2" s="3">
         <v>1</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>1</v>
       </c>
       <c r="Z2" s="2">
         <v>1</v>
       </c>
       <c r="AA2" s="2">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="2">
         <v>244</v>
@@ -1608,11 +1917,14 @@
       <c r="AC2" s="2">
         <v>244</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AD2" s="2">
+        <v>244</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="49" t="s">
         <v>92</v>
       </c>
@@ -1620,19 +1932,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="50">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D3" s="50">
         <v>6</v>
       </c>
       <c r="E3" s="50">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F3" s="50">
         <v>32</v>
       </c>
       <c r="G3" s="50">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H3" s="50">
         <v>6</v>
@@ -1650,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="M3" s="50">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="N3" s="50">
         <v>6</v>
@@ -1673,33 +1985,36 @@
       <c r="T3" s="50">
         <v>6</v>
       </c>
-      <c r="W3" s="3">
-        <f>W2+1</f>
+      <c r="U3" s="50">
+        <v>32</v>
+      </c>
+      <c r="X3" s="3">
+        <f>X2+1</f>
         <v>2</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>2</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>5</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>204</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AC3" s="2">
         <v>185</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AD3" s="2">
         <v>141</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
@@ -1707,49 +2022,49 @@
         <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D4" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F4" s="6">
         <v>19</v>
       </c>
       <c r="G4" s="6">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="H4" s="6">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6">
+        <v>32</v>
+      </c>
+      <c r="J4" s="6">
         <v>5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
+        <v>4</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>4</v>
+      </c>
+      <c r="O4" s="6">
         <v>16</v>
       </c>
-      <c r="J4" s="6">
-        <v>4</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="P4" s="6">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="6">
         <v>37</v>
-      </c>
-      <c r="L4" s="6">
-        <v>32</v>
-      </c>
-      <c r="M4" s="6">
-        <v>6</v>
-      </c>
-      <c r="N4" s="6">
-        <v>15</v>
-      </c>
-      <c r="O4" s="6">
-        <v>5</v>
-      </c>
-      <c r="P4" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>3</v>
       </c>
       <c r="R4" s="6">
         <v>3</v>
@@ -1758,35 +2073,38 @@
         <v>3</v>
       </c>
       <c r="T4" s="6">
-        <v>4</v>
-      </c>
-      <c r="W4" s="3">
-        <f t="shared" ref="W4:W42" si="0">W3+1</f>
         <v>3</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="U4" s="6">
+        <v>6</v>
+      </c>
+      <c r="X4" s="3">
+        <f t="shared" ref="X4:X42" si="0">X3+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Z4" s="2">
         <v>3</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AA4" s="2">
         <v>21</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AB4" s="2">
         <v>180</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0</v>
       </c>
       <c r="AC4" s="2">
         <v>0</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AD4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
@@ -1794,49 +2112,49 @@
         <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6">
         <v>21</v>
       </c>
       <c r="E5" s="6">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="F5" s="6">
         <v>20</v>
       </c>
       <c r="G5" s="6">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H5" s="6">
+        <v>18</v>
+      </c>
+      <c r="I5" s="6">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6">
         <v>3</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6">
+        <v>21</v>
+      </c>
+      <c r="M5" s="6">
+        <v>3</v>
+      </c>
+      <c r="N5" s="6">
+        <v>13</v>
+      </c>
+      <c r="O5" s="6">
         <v>11</v>
       </c>
-      <c r="J5" s="6">
-        <v>14</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="P5" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="6">
         <v>29</v>
-      </c>
-      <c r="L5" s="6">
-        <v>5</v>
-      </c>
-      <c r="M5" s="6">
-        <v>29</v>
-      </c>
-      <c r="N5" s="6">
-        <v>18</v>
-      </c>
-      <c r="O5" s="6">
-        <v>21</v>
-      </c>
-      <c r="P5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>14</v>
       </c>
       <c r="R5" s="6">
         <v>14</v>
@@ -1845,35 +2163,38 @@
         <v>14</v>
       </c>
       <c r="T5" s="6">
-        <v>13</v>
-      </c>
-      <c r="W5" s="3">
+        <v>14</v>
+      </c>
+      <c r="U5" s="6">
+        <v>29</v>
+      </c>
+      <c r="X5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="Y5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>4</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>23</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>30</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AC5" s="2">
         <v>90</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AD5" s="2">
         <v>168</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -1881,86 +2202,89 @@
         <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D6" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E6" s="6">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F6" s="6">
         <v>21</v>
       </c>
       <c r="G6" s="6">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="H6" s="6">
+        <v>40</v>
+      </c>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6">
         <v>29</v>
       </c>
-      <c r="I6" s="6">
+      <c r="K6" s="6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="6">
+        <v>9</v>
+      </c>
+      <c r="N6" s="6">
+        <v>21</v>
+      </c>
+      <c r="O6" s="6">
         <v>18</v>
       </c>
-      <c r="J6" s="6">
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
         <v>5</v>
       </c>
-      <c r="K6" s="6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="6">
-        <v>4</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="S6" s="6">
+        <v>29</v>
+      </c>
+      <c r="T6" s="6">
+        <v>5</v>
+      </c>
+      <c r="U6" s="6">
         <v>25</v>
       </c>
-      <c r="N6" s="6">
-        <v>40</v>
-      </c>
-      <c r="O6" s="6">
-        <v>3</v>
-      </c>
-      <c r="P6" s="6">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>5</v>
-      </c>
-      <c r="R6" s="6">
-        <v>29</v>
-      </c>
-      <c r="S6" s="6">
-        <v>5</v>
-      </c>
-      <c r="T6" s="6">
-        <v>21</v>
-      </c>
-      <c r="W6" s="3">
+      <c r="X6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="X6" s="45" t="s">
+      <c r="Y6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Z6" s="2">
         <v>5</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>24</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <v>250</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AC6" s="2">
         <v>200</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AD6" s="2">
         <v>10</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>93</v>
       </c>
@@ -1968,86 +2292,89 @@
         <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6">
         <v>15</v>
       </c>
       <c r="E7" s="6">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6">
         <v>29</v>
       </c>
       <c r="G7" s="6">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="H7" s="6">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6">
+        <v>3</v>
+      </c>
+      <c r="J7" s="6">
         <v>6</v>
       </c>
-      <c r="I7" s="6">
+      <c r="K7" s="6">
+        <v>5</v>
+      </c>
+      <c r="L7" s="6">
+        <v>15</v>
+      </c>
+      <c r="M7" s="6">
+        <v>18</v>
+      </c>
+      <c r="N7" s="6">
+        <v>24</v>
+      </c>
+      <c r="O7" s="6">
         <v>27</v>
       </c>
-      <c r="J7" s="6">
+      <c r="P7" s="6">
         <v>3</v>
       </c>
-      <c r="K7" s="6">
+      <c r="Q7" s="6">
         <v>21</v>
       </c>
-      <c r="L7" s="6">
-        <v>3</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="R7" s="6">
+        <v>7</v>
+      </c>
+      <c r="S7" s="6">
+        <v>5</v>
+      </c>
+      <c r="T7" s="6">
+        <v>7</v>
+      </c>
+      <c r="U7" s="6">
         <v>10</v>
       </c>
-      <c r="N7" s="6">
-        <v>11</v>
-      </c>
-      <c r="O7" s="6">
-        <v>15</v>
-      </c>
-      <c r="P7" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>7</v>
-      </c>
-      <c r="R7" s="6">
-        <v>5</v>
-      </c>
-      <c r="S7" s="6">
-        <v>7</v>
-      </c>
-      <c r="T7" s="6">
-        <v>24</v>
-      </c>
-      <c r="W7" s="3">
+      <c r="X7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="Y7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <v>6</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>26</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <v>27</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AC7" s="2">
         <v>42</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AD7" s="2">
         <v>52</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>93</v>
       </c>
@@ -2055,86 +2382,89 @@
         <v>14</v>
       </c>
       <c r="C8" s="6">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D8" s="6">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="6">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6">
         <v>39</v>
       </c>
       <c r="G8" s="6">
+        <v>5</v>
+      </c>
+      <c r="H8" s="6">
+        <v>27</v>
+      </c>
+      <c r="I8" s="6">
+        <v>6</v>
+      </c>
+      <c r="J8" s="6">
+        <v>31</v>
+      </c>
+      <c r="K8" s="6">
+        <v>10</v>
+      </c>
+      <c r="L8" s="6">
+        <v>22</v>
+      </c>
+      <c r="M8" s="6">
+        <v>26</v>
+      </c>
+      <c r="N8" s="6">
+        <v>26</v>
+      </c>
+      <c r="O8" s="6">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>31</v>
+      </c>
+      <c r="R8" s="6">
+        <v>4</v>
+      </c>
+      <c r="S8" s="6">
         <v>15</v>
       </c>
-      <c r="H8" s="6">
-        <v>31</v>
-      </c>
-      <c r="I8" s="6">
-        <v>17</v>
-      </c>
-      <c r="J8" s="6">
-        <v>9</v>
-      </c>
-      <c r="K8" s="6">
-        <v>31</v>
-      </c>
-      <c r="L8" s="6">
-        <v>6</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="T8" s="6">
+        <v>4</v>
+      </c>
+      <c r="U8" s="6">
         <v>32</v>
       </c>
-      <c r="N8" s="6">
-        <v>27</v>
-      </c>
-      <c r="O8" s="6">
-        <v>14</v>
-      </c>
-      <c r="P8" s="6">
-        <v>10</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>4</v>
-      </c>
-      <c r="R8" s="6">
-        <v>15</v>
-      </c>
-      <c r="S8" s="6">
-        <v>4</v>
-      </c>
-      <c r="T8" s="6">
-        <v>26</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="X8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="X8" s="11" t="s">
+      <c r="Y8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <v>7</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
         <v>28</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <v>0</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AC8" s="2">
         <v>133</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AD8" s="2">
         <v>43</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>93</v>
       </c>
@@ -2142,86 +2472,89 @@
         <v>20</v>
       </c>
       <c r="C9" s="6">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D9" s="6">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6">
         <v>22</v>
       </c>
       <c r="G9" s="6">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H9" s="6">
+        <v>3</v>
+      </c>
+      <c r="I9" s="6">
+        <v>19</v>
+      </c>
+      <c r="J9" s="6">
         <v>9</v>
       </c>
-      <c r="I9" s="6">
+      <c r="K9" s="6">
+        <v>6</v>
+      </c>
+      <c r="L9" s="6">
+        <v>17</v>
+      </c>
+      <c r="M9" s="6">
+        <v>15</v>
+      </c>
+      <c r="N9" s="6">
+        <v>30</v>
+      </c>
+      <c r="O9" s="6">
         <v>2</v>
       </c>
-      <c r="J9" s="6">
-        <v>36</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="P9" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="6">
         <v>39</v>
       </c>
-      <c r="L9" s="6">
-        <v>19</v>
-      </c>
-      <c r="M9" s="6">
+      <c r="R9" s="6">
+        <v>32</v>
+      </c>
+      <c r="S9" s="6">
+        <v>7</v>
+      </c>
+      <c r="T9" s="6">
+        <v>32</v>
+      </c>
+      <c r="U9" s="6">
         <v>5</v>
       </c>
-      <c r="N9" s="6">
-        <v>3</v>
-      </c>
-      <c r="O9" s="6">
-        <v>4</v>
-      </c>
-      <c r="P9" s="6">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>32</v>
-      </c>
-      <c r="R9" s="6">
-        <v>7</v>
-      </c>
-      <c r="S9" s="6">
-        <v>32</v>
-      </c>
-      <c r="T9" s="6">
-        <v>30</v>
-      </c>
-      <c r="W9" s="3">
+      <c r="X9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="X9" s="46" t="s">
+      <c r="Y9" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>8</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>192</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <v>95</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <v>49</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AD9" s="2">
         <v>9</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>93</v>
       </c>
@@ -2229,74 +2562,74 @@
         <v>13</v>
       </c>
       <c r="C10" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E10" s="6">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F10" s="6">
         <v>41</v>
       </c>
       <c r="G10" s="6">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="H10" s="6">
         <v>17</v>
       </c>
       <c r="I10" s="6">
+        <v>29</v>
+      </c>
+      <c r="J10" s="6">
+        <v>17</v>
+      </c>
+      <c r="K10" s="6">
+        <v>16</v>
+      </c>
+      <c r="L10" s="6">
+        <v>3</v>
+      </c>
+      <c r="M10" s="6">
+        <v>8</v>
+      </c>
+      <c r="N10" s="6">
+        <v>36</v>
+      </c>
+      <c r="O10" s="6">
         <v>4</v>
       </c>
-      <c r="J10" s="6">
-        <v>7</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="P10" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="6">
         <v>36</v>
       </c>
-      <c r="L10" s="6">
-        <v>29</v>
-      </c>
-      <c r="M10" s="6">
+      <c r="R10" s="6">
+        <v>38</v>
+      </c>
+      <c r="S10" s="6">
+        <v>24</v>
+      </c>
+      <c r="T10" s="6">
+        <v>38</v>
+      </c>
+      <c r="U10" s="6">
         <v>19</v>
       </c>
-      <c r="N10" s="6">
-        <v>17</v>
-      </c>
-      <c r="O10" s="6">
-        <v>20</v>
-      </c>
-      <c r="P10" s="6">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>38</v>
-      </c>
-      <c r="R10" s="6">
-        <v>24</v>
-      </c>
-      <c r="S10" s="6">
-        <v>38</v>
-      </c>
-      <c r="T10" s="6">
-        <v>36</v>
-      </c>
-      <c r="W10" s="3">
+      <c r="X10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="X10" s="12" t="s">
+      <c r="Y10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <v>9</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AA10" s="2">
         <v>194</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>150</v>
       </c>
       <c r="AB10" s="2">
         <v>150</v>
@@ -2304,11 +2637,14 @@
       <c r="AC10" s="2">
         <v>150</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AD10" s="2">
+        <v>150</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>93</v>
       </c>
@@ -2316,72 +2652,72 @@
         <v>18</v>
       </c>
       <c r="C11" s="6">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D11" s="6">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E11" s="6">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F11" s="6">
         <v>24</v>
       </c>
       <c r="G11" s="6">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6">
+        <v>39</v>
+      </c>
+      <c r="I11" s="6">
+        <v>24</v>
+      </c>
+      <c r="J11" s="6">
+        <v>10</v>
+      </c>
+      <c r="K11" s="6">
+        <v>17</v>
+      </c>
+      <c r="L11" s="6">
+        <v>13</v>
+      </c>
+      <c r="M11" s="6">
+        <v>14</v>
+      </c>
+      <c r="N11" s="6">
+        <v>37</v>
+      </c>
+      <c r="O11" s="6">
+        <v>35</v>
+      </c>
+      <c r="P11" s="6">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>33</v>
+      </c>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6">
         <v>21</v>
       </c>
-      <c r="H11" s="6">
-        <v>10</v>
-      </c>
-      <c r="I11" s="6">
-        <v>35</v>
-      </c>
-      <c r="J11" s="6">
+      <c r="T11" s="6">
+        <v>19</v>
+      </c>
+      <c r="U11" s="6">
         <v>18</v>
       </c>
-      <c r="K11" s="6">
-        <v>33</v>
-      </c>
-      <c r="L11" s="6">
-        <v>24</v>
-      </c>
-      <c r="M11" s="6">
-        <v>18</v>
-      </c>
-      <c r="N11" s="6">
-        <v>39</v>
-      </c>
-      <c r="O11" s="6">
-        <v>1</v>
-      </c>
-      <c r="P11" s="6">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6">
-        <v>21</v>
-      </c>
-      <c r="S11" s="6">
-        <v>19</v>
-      </c>
-      <c r="T11" s="6">
-        <v>37</v>
-      </c>
-      <c r="W11" s="3">
+      <c r="X11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="X11" s="13" t="s">
+      <c r="Y11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <v>10</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AA11" s="2">
         <v>199</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>100</v>
       </c>
       <c r="AB11" s="2">
         <v>100</v>
@@ -2389,11 +2725,14 @@
       <c r="AC11" s="2">
         <v>100</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AD11" s="2">
+        <v>100</v>
+      </c>
+      <c r="AE11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>93</v>
       </c>
@@ -2401,82 +2740,85 @@
         <v>12</v>
       </c>
       <c r="C12" s="6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E12" s="6">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F12" s="6">
         <v>25</v>
       </c>
       <c r="G12" s="6">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H12" s="6">
+        <v>35</v>
+      </c>
+      <c r="I12" s="6">
+        <v>25</v>
+      </c>
+      <c r="J12" s="6">
         <v>32</v>
       </c>
-      <c r="I12" s="6">
+      <c r="K12" s="6">
+        <v>29</v>
+      </c>
+      <c r="L12" s="6">
+        <v>16</v>
+      </c>
+      <c r="M12" s="6">
+        <v>2</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6">
         <v>41</v>
       </c>
-      <c r="J12" s="6">
-        <v>10</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="P12" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="6">
         <v>41</v>
       </c>
-      <c r="L12" s="6">
-        <v>25</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="R12" s="6"/>
+      <c r="S12" s="6">
+        <v>4</v>
+      </c>
+      <c r="T12" s="6">
+        <v>29</v>
+      </c>
+      <c r="U12" s="6">
         <v>31</v>
       </c>
-      <c r="N12" s="6">
-        <v>35</v>
-      </c>
-      <c r="O12" s="6">
-        <v>29</v>
-      </c>
-      <c r="P12" s="6">
-        <v>29</v>
-      </c>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6">
-        <v>4</v>
-      </c>
-      <c r="S12" s="6">
-        <v>29</v>
-      </c>
-      <c r="T12" s="6"/>
-      <c r="W12" s="3">
+      <c r="X12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="X12" s="14" t="s">
+      <c r="Y12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Z12" s="2">
         <v>11</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AA12" s="2">
         <v>18</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>187</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AC12" s="2">
         <v>128</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AD12" s="2">
         <v>90</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AE12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>93</v>
       </c>
@@ -2484,82 +2826,85 @@
         <v>10</v>
       </c>
       <c r="C13" s="6">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="6">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E13" s="6">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6">
         <v>31</v>
       </c>
       <c r="G13" s="6">
+        <v>11</v>
+      </c>
+      <c r="H13" s="6">
+        <v>31</v>
+      </c>
+      <c r="I13" s="6">
+        <v>39</v>
+      </c>
+      <c r="J13" s="6">
+        <v>2</v>
+      </c>
+      <c r="K13" s="6">
+        <v>19</v>
+      </c>
+      <c r="L13" s="6">
+        <v>17</v>
+      </c>
+      <c r="M13" s="6">
+        <v>29</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6">
+        <v>40</v>
+      </c>
+      <c r="P13" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>30</v>
+      </c>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6">
         <v>32</v>
       </c>
-      <c r="H13" s="6">
-        <v>2</v>
-      </c>
-      <c r="I13" s="6">
-        <v>40</v>
-      </c>
-      <c r="J13" s="6">
-        <v>21</v>
-      </c>
-      <c r="K13" s="6">
-        <v>30</v>
-      </c>
-      <c r="L13" s="6">
-        <v>39</v>
-      </c>
-      <c r="M13" s="6">
+      <c r="T13" s="6">
+        <v>15</v>
+      </c>
+      <c r="U13" s="6">
         <v>24</v>
       </c>
-      <c r="N13" s="6">
-        <v>31</v>
-      </c>
-      <c r="O13" s="6">
-        <v>32</v>
-      </c>
-      <c r="P13" s="6">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6">
-        <v>32</v>
-      </c>
-      <c r="S13" s="6">
-        <v>15</v>
-      </c>
-      <c r="T13" s="6"/>
-      <c r="W13" s="3">
+      <c r="X13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="X13" s="15" t="s">
+      <c r="Y13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Z13" s="2">
         <v>12</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AA13" s="2">
         <v>37</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AB13" s="2">
         <v>88</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AC13" s="2">
         <v>171</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AD13" s="2">
         <v>65</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>93</v>
       </c>
@@ -2567,82 +2912,85 @@
         <v>21</v>
       </c>
       <c r="C14" s="6">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F14" s="6">
         <v>30</v>
       </c>
       <c r="G14" s="6">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="H14" s="6">
+        <v>7</v>
+      </c>
+      <c r="I14" s="6">
+        <v>41</v>
+      </c>
+      <c r="J14" s="6">
         <v>14</v>
       </c>
-      <c r="I14" s="6">
+      <c r="K14" s="6">
+        <v>18</v>
+      </c>
+      <c r="L14" s="6">
+        <v>18</v>
+      </c>
+      <c r="M14" s="6">
+        <v>32</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6">
         <v>26</v>
       </c>
-      <c r="J14" s="6">
-        <v>29</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="P14" s="6">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="6">
         <v>35</v>
       </c>
-      <c r="L14" s="6">
-        <v>41</v>
-      </c>
-      <c r="M14" s="6">
+      <c r="R14" s="6"/>
+      <c r="S14" s="6">
+        <v>25</v>
+      </c>
+      <c r="T14" s="6">
+        <v>24</v>
+      </c>
+      <c r="U14" s="6">
         <v>38</v>
       </c>
-      <c r="N14" s="6">
-        <v>7</v>
-      </c>
-      <c r="O14" s="6">
-        <v>19</v>
-      </c>
-      <c r="P14" s="6">
-        <v>18</v>
-      </c>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6">
-        <v>25</v>
-      </c>
-      <c r="S14" s="6">
-        <v>24</v>
-      </c>
-      <c r="T14" s="6"/>
-      <c r="W14" s="3">
+      <c r="X14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="X14" s="16" t="s">
+      <c r="Y14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Z14" s="2">
         <v>13</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AA14" s="2">
         <v>102</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AB14" s="2">
         <v>115</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AC14" s="2">
         <v>150</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AD14" s="2">
         <v>200</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>93</v>
       </c>
@@ -2650,222 +2998,235 @@
         <v>15</v>
       </c>
       <c r="C15" s="6">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D15" s="6">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E15" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="6">
         <v>15</v>
       </c>
       <c r="G15" s="6">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H15" s="6">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6">
+        <v>36</v>
+      </c>
+      <c r="J15" s="6">
         <v>41</v>
       </c>
-      <c r="I15" s="6">
-        <v>39</v>
-      </c>
-      <c r="J15" s="6">
-        <v>39</v>
-      </c>
       <c r="K15" s="6">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="L15" s="6">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M15" s="6">
-        <v>36</v>
-      </c>
-      <c r="N15" s="6">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="N15" s="6"/>
       <c r="O15" s="6">
         <v>39</v>
       </c>
       <c r="P15" s="6">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>24</v>
+      </c>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6">
         <v>19</v>
       </c>
-      <c r="S15" s="6">
+      <c r="T15" s="6">
         <v>21</v>
       </c>
-      <c r="T15" s="6"/>
-      <c r="W15" s="3">
+      <c r="U15" s="6">
+        <v>36</v>
+      </c>
+      <c r="X15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="X15" s="17" t="s">
+      <c r="Y15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Z15" s="2">
         <v>14</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AA15" s="2">
         <v>106</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AB15" s="2">
         <v>214</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AC15" s="2">
         <v>121</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AD15" s="2">
         <v>35</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="6">
         <v>22</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6">
+        <v>6</v>
+      </c>
       <c r="D16" s="6">
-        <v>36</v>
-      </c>
-      <c r="E16" s="6">
-        <v>35</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="6">
         <v>14</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6">
+        <v>26</v>
+      </c>
       <c r="H16" s="6">
+        <v>28</v>
+      </c>
+      <c r="I16" s="6">
+        <v>21</v>
+      </c>
+      <c r="J16" s="6">
         <v>16</v>
       </c>
-      <c r="I16" s="6">
+      <c r="K16" s="6">
+        <v>30</v>
+      </c>
+      <c r="L16" s="6">
+        <v>36</v>
+      </c>
+      <c r="M16" s="6">
+        <v>35</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6">
         <v>31</v>
       </c>
-      <c r="J16" s="6">
-        <v>6</v>
-      </c>
-      <c r="K16" s="6">
+      <c r="P16" s="6">
+        <v>39</v>
+      </c>
+      <c r="Q16" s="6">
         <v>26</v>
       </c>
-      <c r="L16" s="6">
-        <v>21</v>
-      </c>
-      <c r="M16" s="6">
+      <c r="R16" s="6"/>
+      <c r="S16" s="6">
+        <v>20</v>
+      </c>
+      <c r="T16" s="6">
+        <v>25</v>
+      </c>
+      <c r="U16" s="6">
         <v>17</v>
       </c>
-      <c r="N16" s="6">
-        <v>28</v>
-      </c>
-      <c r="O16" s="6">
-        <v>41</v>
-      </c>
-      <c r="P16" s="6">
-        <v>30</v>
-      </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6">
-        <v>20</v>
-      </c>
-      <c r="S16" s="6">
-        <v>25</v>
-      </c>
-      <c r="T16" s="6"/>
-      <c r="W16" s="3">
+      <c r="X16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="X16" s="18" t="s">
+      <c r="Y16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="2">
         <v>15</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AA16" s="2">
         <v>119</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AB16" s="2">
         <v>165</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AC16" s="2">
         <v>202</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AD16" s="2">
         <v>24</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B17" s="6">
         <v>29</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6">
+        <v>13</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6">
+        <v>27</v>
+      </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6">
-        <v>13</v>
-      </c>
-      <c r="K17" s="6">
-        <v>28</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="I17" s="6">
         <v>20</v>
       </c>
-      <c r="M17" s="6">
-        <v>40</v>
-      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="P17" s="6">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>28</v>
+      </c>
       <c r="R17" s="6"/>
-      <c r="S17" s="6">
+      <c r="S17" s="6"/>
+      <c r="T17" s="6">
         <v>20</v>
       </c>
-      <c r="T17" s="6"/>
-      <c r="W17" s="3">
+      <c r="U17" s="6">
+        <v>40</v>
+      </c>
+      <c r="X17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="X17" s="42" t="s">
+      <c r="Y17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Z17" s="2">
         <v>16</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AA17" s="2">
         <v>140</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AB17" s="2">
         <v>25</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="AC17" s="2">
         <v>50</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="AD17" s="2">
         <v>90</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>93</v>
       </c>
@@ -2876,7 +3237,9 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="G18" s="6">
+        <v>28</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -2888,37 +3251,38 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="6">
+      <c r="S18" s="6"/>
+      <c r="T18" s="6">
         <v>18</v>
       </c>
-      <c r="T18" s="6"/>
-      <c r="W18" s="3">
+      <c r="U18" s="6"/>
+      <c r="X18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="X18" s="43" t="s">
+      <c r="Y18" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Z18" s="2">
         <v>17</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="AA18" s="2">
         <v>141</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AB18" s="2">
         <v>0</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="AC18" s="2">
         <v>69</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="AD18" s="2">
         <v>26</v>
       </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AE18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>93</v>
       </c>
@@ -2943,33 +3307,34 @@
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
-      <c r="W19" s="3">
+      <c r="U19" s="6"/>
+      <c r="X19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="X19" s="44" t="s">
+      <c r="Y19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Z19" s="2">
         <v>18</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AA19" s="2">
         <v>154</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AB19" s="2">
         <v>114</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="AC19" s="2">
         <v>0</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="AD19" s="2">
         <v>18</v>
       </c>
-      <c r="AD19" s="2" t="s">
+      <c r="AE19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
@@ -2994,33 +3359,34 @@
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
-      <c r="W20" s="3">
+      <c r="U20" s="6"/>
+      <c r="X20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X20" s="19" t="s">
+      <c r="Y20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Z20" s="2">
         <v>19</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AA20" s="2">
         <v>221</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AB20" s="2">
         <v>200</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AC20" s="2">
         <v>80</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="AD20" s="2">
         <v>155</v>
       </c>
-      <c r="AD20" s="2" t="s">
+      <c r="AE20" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>93</v>
       </c>
@@ -3045,33 +3411,34 @@
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
-      <c r="W21" s="3">
+      <c r="U21" s="6"/>
+      <c r="X21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="X21" s="20" t="s">
+      <c r="Y21" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Z21" s="2">
         <v>20</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AA21" s="2">
         <v>222</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AB21" s="2">
         <v>255</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="AC21" s="2">
         <v>158</v>
       </c>
-      <c r="AC21" s="2">
+      <c r="AD21" s="2">
         <v>205</v>
       </c>
-      <c r="AD21" s="2" t="s">
+      <c r="AE21" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>93</v>
       </c>
@@ -3096,33 +3463,34 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
-      <c r="W22" s="3">
+      <c r="U22" s="6"/>
+      <c r="X22" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="X22" s="21" t="s">
+      <c r="Y22" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="Z22" s="2">
         <v>21</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="AA22" s="2">
         <v>322</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="AB22" s="2">
         <v>104</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="AC22" s="2">
         <v>195</v>
       </c>
-      <c r="AC22" s="2">
+      <c r="AD22" s="2">
         <v>226</v>
       </c>
-      <c r="AD22" s="2" t="s">
+      <c r="AE22" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>93</v>
       </c>
@@ -3147,33 +3515,34 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-      <c r="W23" s="3">
+      <c r="U23" s="6"/>
+      <c r="X23" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="X23" s="22" t="s">
+      <c r="Y23" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Z23" s="2">
         <v>22</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AA23" s="2">
         <v>324</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AB23" s="2">
         <v>154</v>
       </c>
-      <c r="AB23" s="2">
+      <c r="AC23" s="2">
         <v>118</v>
       </c>
-      <c r="AC23" s="2">
+      <c r="AD23" s="2">
         <v>174</v>
       </c>
-      <c r="AD23" s="2" t="s">
+      <c r="AE23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
@@ -3198,33 +3567,34 @@
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="W24" s="3">
+      <c r="U24" s="6"/>
+      <c r="X24" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="X24" s="23" t="s">
+      <c r="Y24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Z24" s="2">
         <v>23</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="AA24" s="2">
         <v>38</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="AB24" s="2">
         <v>145</v>
       </c>
-      <c r="AB24" s="2">
+      <c r="AC24" s="2">
         <v>80</v>
       </c>
-      <c r="AC24" s="2">
+      <c r="AD24" s="2">
         <v>28</v>
       </c>
-      <c r="AD24" s="2" t="s">
+      <c r="AE24" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
@@ -3249,621 +3619,753 @@
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
-      <c r="W25" s="3">
+      <c r="U25" s="6"/>
+      <c r="X25" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="X25" s="24" t="s">
+      <c r="Y25" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="Y25" s="2">
+      <c r="Z25" s="2">
         <v>24</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AA25" s="2">
         <v>107</v>
       </c>
-      <c r="AA25" s="2">
+      <c r="AB25" s="2">
         <v>0</v>
       </c>
-      <c r="AB25" s="2">
+      <c r="AC25" s="2">
         <v>152</v>
       </c>
-      <c r="AC25" s="2">
+      <c r="AD25" s="2">
         <v>148</v>
       </c>
-      <c r="AD25" s="2" t="s">
+      <c r="AE25" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W26" s="3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X26" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="X26" s="25" t="s">
+      <c r="Y26" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="Z26" s="2">
         <v>25</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="AA26" s="2">
         <v>124</v>
       </c>
-      <c r="AA26" s="2">
+      <c r="AB26" s="2">
         <v>144</v>
       </c>
-      <c r="AB26" s="2">
+      <c r="AC26" s="2">
         <v>31</v>
       </c>
-      <c r="AC26" s="2">
+      <c r="AD26" s="2">
         <v>118</v>
       </c>
-      <c r="AD26" s="2" t="s">
+      <c r="AE26" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W27" s="3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X27" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="X27" s="26" t="s">
+      <c r="Y27" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="Z27" s="2">
         <v>26</v>
       </c>
-      <c r="Z27" s="2">
+      <c r="AA27" s="2">
         <v>135</v>
       </c>
-      <c r="AA27" s="2">
+      <c r="AB27" s="2">
         <v>112</v>
       </c>
-      <c r="AB27" s="2">
+      <c r="AC27" s="2">
         <v>129</v>
       </c>
-      <c r="AC27" s="2">
+      <c r="AD27" s="2">
         <v>154</v>
       </c>
-      <c r="AD27" s="2" t="s">
+      <c r="AE27" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W28" s="3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X28" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="X28" s="27" t="s">
+      <c r="Y28" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="Z28" s="2">
         <v>27</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="AA28" s="2">
         <v>138</v>
       </c>
-      <c r="AA28" s="2">
+      <c r="AB28" s="2">
         <v>137</v>
       </c>
-      <c r="AB28" s="2">
+      <c r="AC28" s="2">
         <v>125</v>
       </c>
-      <c r="AC28" s="2">
+      <c r="AD28" s="2">
         <v>98</v>
       </c>
-      <c r="AD28" s="2" t="s">
+      <c r="AE28" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W29" s="3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X29" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="X29" s="28" t="s">
+      <c r="Y29" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="Z29" s="2">
         <v>28</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="AA29" s="2">
         <v>151</v>
       </c>
-      <c r="AA29" s="2">
+      <c r="AB29" s="2">
         <v>112</v>
       </c>
-      <c r="AB29" s="2">
+      <c r="AC29" s="2">
         <v>142</v>
       </c>
-      <c r="AC29" s="2">
+      <c r="AD29" s="2">
         <v>124</v>
       </c>
-      <c r="AD29" s="2" t="s">
+      <c r="AE29" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W30" s="3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X30" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="X30" s="29" t="s">
+      <c r="Y30" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="Z30" s="2">
         <v>29</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="AA30" s="2">
         <v>191</v>
       </c>
-      <c r="AA30" s="2">
+      <c r="AB30" s="2">
         <v>252</v>
       </c>
-      <c r="AB30" s="2">
+      <c r="AC30" s="2">
         <v>172</v>
       </c>
-      <c r="AC30" s="2">
+      <c r="AD30" s="2">
         <v>0</v>
       </c>
-      <c r="AD30" s="2" t="s">
+      <c r="AE30" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W31" s="3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X31" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="X31" s="30" t="s">
+      <c r="Y31" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="Z31" s="2">
         <v>30</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="AA31" s="2">
         <v>212</v>
       </c>
-      <c r="AA31" s="2">
+      <c r="AB31" s="2">
         <v>157</v>
       </c>
-      <c r="AB31" s="2">
+      <c r="AC31" s="2">
         <v>195</v>
       </c>
-      <c r="AC31" s="2">
+      <c r="AD31" s="2">
         <v>247</v>
       </c>
-      <c r="AD31" s="2" t="s">
+      <c r="AE31" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="W32" s="3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="X32" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="X32" s="31" t="s">
+      <c r="Y32" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="Z32" s="2">
         <v>31</v>
       </c>
-      <c r="Z32" s="2">
+      <c r="AA32" s="2">
         <v>226</v>
       </c>
-      <c r="AA32" s="2">
+      <c r="AB32" s="2">
         <v>255</v>
       </c>
-      <c r="AB32" s="2">
+      <c r="AC32" s="2">
         <v>236</v>
       </c>
-      <c r="AC32" s="2">
+      <c r="AD32" s="2">
         <v>108</v>
       </c>
-      <c r="AD32" s="2" t="s">
+      <c r="AE32" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W33" s="3">
+    <row r="33" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X33" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="X33" s="41" t="s">
+      <c r="Y33" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="Z33" s="2">
         <v>32</v>
       </c>
-      <c r="Z33" s="2">
+      <c r="AA33" s="2">
         <v>268</v>
       </c>
-      <c r="AA33" s="2">
+      <c r="AB33" s="2">
         <v>68</v>
       </c>
-      <c r="AB33" s="2">
+      <c r="AC33" s="2">
         <v>26</v>
       </c>
-      <c r="AC33" s="2">
+      <c r="AD33" s="2">
         <v>145</v>
       </c>
-      <c r="AD33" s="2" t="s">
+      <c r="AE33" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W34" s="3">
+    <row r="34" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X34" s="3">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="X34" s="32" t="s">
+      <c r="Y34" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="Z34" s="2">
         <v>33</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="AA34" s="2">
         <v>283</v>
       </c>
-      <c r="AA34" s="2">
+      <c r="AB34" s="2">
         <v>225</v>
       </c>
-      <c r="AB34" s="2">
+      <c r="AC34" s="2">
         <v>190</v>
       </c>
-      <c r="AC34" s="2">
+      <c r="AD34" s="2">
         <v>161</v>
       </c>
-      <c r="AD34" s="2" t="s">
+      <c r="AE34" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W35" s="3">
+    <row r="35" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X35" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="X35" s="33" t="s">
+      <c r="Y35" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="Z35" s="2">
         <v>34</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="AA35" s="2">
         <v>308</v>
       </c>
-      <c r="AA35" s="2">
+      <c r="AB35" s="2">
         <v>53</v>
       </c>
-      <c r="AB35" s="2">
+      <c r="AC35" s="2">
         <v>33</v>
       </c>
-      <c r="AC35" s="2">
+      <c r="AD35" s="2">
         <v>0</v>
       </c>
-      <c r="AD35" s="2" t="s">
+      <c r="AE35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W36" s="3">
+    <row r="36" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X36" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="X36" s="34" t="s">
+      <c r="Y36" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="Z36" s="2">
         <v>35</v>
       </c>
-      <c r="Z36" s="2">
+      <c r="AA36" s="2">
         <v>312</v>
       </c>
-      <c r="AA36" s="2">
+      <c r="AB36" s="2">
         <v>170</v>
       </c>
-      <c r="AB36" s="2">
+      <c r="AC36" s="2">
         <v>125</v>
       </c>
-      <c r="AC36" s="2">
+      <c r="AD36" s="2">
         <v>85</v>
       </c>
-      <c r="AD36" s="2" t="s">
+      <c r="AE36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W37" s="3">
+    <row r="37" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X37" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="X37" s="37" t="s">
+      <c r="Y37" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="Y37" s="2">
+      <c r="Z37" s="2">
         <v>36</v>
       </c>
-      <c r="Z37" s="2">
+      <c r="AA37" s="2">
         <v>321</v>
       </c>
-      <c r="AA37" s="2">
+      <c r="AB37" s="2">
         <v>70</v>
       </c>
-      <c r="AB37" s="2">
+      <c r="AC37" s="2">
         <v>155</v>
       </c>
-      <c r="AC37" s="2">
+      <c r="AD37" s="2">
         <v>195</v>
       </c>
-      <c r="AD37" s="2" t="s">
+      <c r="AE37" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W38" s="3">
+    <row r="38" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X38" s="3">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="X38" s="38" t="s">
+      <c r="Y38" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="Y38" s="2">
+      <c r="Z38" s="2">
         <v>37</v>
       </c>
-      <c r="Z38" s="2">
+      <c r="AA38" s="2">
         <v>323</v>
       </c>
-      <c r="AA38" s="2">
+      <c r="AB38" s="2">
         <v>211</v>
       </c>
-      <c r="AB38" s="2">
+      <c r="AC38" s="2">
         <v>242</v>
       </c>
-      <c r="AC38" s="2">
+      <c r="AD38" s="2">
         <v>234</v>
       </c>
-      <c r="AD38" s="2" t="s">
+      <c r="AE38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W39" s="3">
+    <row r="39" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X39" s="3">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="X39" s="39" t="s">
+      <c r="Y39" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="Y39" s="2">
+      <c r="Z39" s="2">
         <v>38</v>
       </c>
-      <c r="Z39" s="2">
+      <c r="AA39" s="2">
         <v>325</v>
       </c>
-      <c r="AA39" s="2">
+      <c r="AB39" s="2">
         <v>205</v>
       </c>
-      <c r="AB39" s="2">
+      <c r="AC39" s="2">
         <v>164</v>
       </c>
-      <c r="AC39" s="2">
+      <c r="AD39" s="2">
         <v>222</v>
       </c>
-      <c r="AD39" s="2" t="s">
+      <c r="AE39" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W40" s="3">
+    <row r="40" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X40" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="X40" s="40" t="s">
+      <c r="Y40" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="Y40" s="2">
+      <c r="Z40" s="2">
         <v>39</v>
       </c>
-      <c r="Z40" s="2">
+      <c r="AA40" s="2">
         <v>326</v>
       </c>
-      <c r="AA40" s="2">
+      <c r="AB40" s="2">
         <v>226</v>
       </c>
-      <c r="AB40" s="2">
+      <c r="AC40" s="2">
         <v>249</v>
       </c>
-      <c r="AC40" s="2">
+      <c r="AD40" s="2">
         <v>154</v>
       </c>
-      <c r="AD40" s="2" t="s">
+      <c r="AE40" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W41" s="3">
+    <row r="41" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X41" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="X41" s="35" t="s">
+      <c r="Y41" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="Y41" s="2">
+      <c r="Z41" s="2">
         <v>40</v>
       </c>
-      <c r="Z41" s="2">
+      <c r="AA41" s="2">
         <v>330</v>
       </c>
-      <c r="AA41" s="2">
+      <c r="AB41" s="2">
         <v>139</v>
       </c>
-      <c r="AB41" s="2">
+      <c r="AC41" s="2">
         <v>132</v>
       </c>
-      <c r="AC41" s="2">
+      <c r="AD41" s="2">
         <v>79</v>
       </c>
-      <c r="AD41" s="2" t="s">
+      <c r="AE41" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="23:30" x14ac:dyDescent="0.35">
-      <c r="W42" s="3">
+    <row r="42" spans="24:31" x14ac:dyDescent="0.3">
+      <c r="X42" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="X42" s="36" t="s">
+      <c r="Y42" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="Y42" s="2">
+      <c r="Z42" s="2">
         <v>41</v>
       </c>
-      <c r="Z42" s="2">
+      <c r="AA42" s="2">
         <v>353</v>
       </c>
-      <c r="AA42" s="2">
+      <c r="AB42" s="2">
         <v>240</v>
       </c>
-      <c r="AB42" s="2">
+      <c r="AC42" s="2">
         <v>109</v>
       </c>
-      <c r="AC42" s="2">
+      <c r="AD42" s="2">
         <v>120</v>
       </c>
-      <c r="AD42" s="2" t="s">
+      <c r="AE42" s="2" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:T25">
-    <cfRule type="expression" dxfId="42" priority="44">
+  <conditionalFormatting sqref="B2:F25">
+    <cfRule type="expression" dxfId="85" priority="87">
       <formula>ISBLANK(B2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="88" stopIfTrue="1">
       <formula>"isblank(B2)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="46" stopIfTrue="1">
-      <formula>B2=$W$2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="47" stopIfTrue="1">
-      <formula>B2=$W$3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="48" stopIfTrue="1">
-      <formula>B2=$W$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="49" stopIfTrue="1">
-      <formula>B2=$W$5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="50" stopIfTrue="1">
-      <formula>B2=$W$6</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="51" stopIfTrue="1">
-      <formula>B2=$W$7</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="52" stopIfTrue="1">
-      <formula>B2=$W$8</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="53" stopIfTrue="1">
-      <formula>B2=$W$9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="54" stopIfTrue="1">
-      <formula>B2=$W$10</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="55" stopIfTrue="1">
-      <formula>B2=$W$11</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="56" stopIfTrue="1">
-      <formula>B2=$W$12</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="57" stopIfTrue="1">
-      <formula>B2=$W$13</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="58" stopIfTrue="1">
-      <formula>B2=$W$14</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="59" stopIfTrue="1">
-      <formula>B2=$W$15</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="60" stopIfTrue="1">
-      <formula>B2=$W$16</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="61" stopIfTrue="1">
-      <formula>B2=$W$17</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="62" stopIfTrue="1">
-      <formula>B2=$W$18</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="63" stopIfTrue="1">
-      <formula>B2=$W$19</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="64" stopIfTrue="1">
-      <formula>B2=$W$20</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="65" stopIfTrue="1">
-      <formula>B2=$W$21</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="66" stopIfTrue="1">
-      <formula>B2=$W$22</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="67" stopIfTrue="1">
-      <formula>B2=$W$23</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="68" stopIfTrue="1">
-      <formula>B2=$W$24</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="69" stopIfTrue="1">
-      <formula>B2=$W$25</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="70" stopIfTrue="1">
-      <formula>B2=$W$26</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="71" stopIfTrue="1">
-      <formula>B2=$W$27</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="72" stopIfTrue="1">
-      <formula>B2=$W$28</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="73" stopIfTrue="1">
-      <formula>B2=$W$29</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="74" stopIfTrue="1">
-      <formula>B2=$W$30</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="75" stopIfTrue="1">
-      <formula>B2=$W$31</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="76" stopIfTrue="1">
-      <formula>B2=$W$32</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="77" stopIfTrue="1">
-      <formula>B2=$W$33</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="78" stopIfTrue="1">
-      <formula>B2=$W$34</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="79" stopIfTrue="1">
-      <formula>B2=$W$35</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="80" stopIfTrue="1">
-      <formula>B2=$W$36</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="81" stopIfTrue="1">
-      <formula>B2=$W$37</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="82" stopIfTrue="1">
-      <formula>B2=$W$38</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="83" stopIfTrue="1">
-      <formula>B2=$W$39</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="84" stopIfTrue="1">
-      <formula>B2=$W$40</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="85" stopIfTrue="1">
-      <formula>B2=$W$41</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="86" stopIfTrue="1">
-      <formula>B2=$W$42</formula>
+    <cfRule type="expression" dxfId="83" priority="89" stopIfTrue="1">
+      <formula>B2=$X$2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="90" stopIfTrue="1">
+      <formula>B2=$X$3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="91" stopIfTrue="1">
+      <formula>B2=$X$4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="92" stopIfTrue="1">
+      <formula>B2=$X$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="93" stopIfTrue="1">
+      <formula>B2=$X$6</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="94" stopIfTrue="1">
+      <formula>B2=$X$7</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="95" stopIfTrue="1">
+      <formula>B2=$X$8</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="96" stopIfTrue="1">
+      <formula>B2=$X$9</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="97" stopIfTrue="1">
+      <formula>B2=$X$10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="98" stopIfTrue="1">
+      <formula>B2=$X$11</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="99" stopIfTrue="1">
+      <formula>B2=$X$12</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="100" stopIfTrue="1">
+      <formula>B2=$X$13</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="101" stopIfTrue="1">
+      <formula>B2=$X$14</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="102" stopIfTrue="1">
+      <formula>B2=$X$15</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="103" stopIfTrue="1">
+      <formula>B2=$X$16</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="104" stopIfTrue="1">
+      <formula>B2=$X$17</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="105" stopIfTrue="1">
+      <formula>B2=$X$18</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="106" stopIfTrue="1">
+      <formula>B2=$X$19</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="107" stopIfTrue="1">
+      <formula>B2=$X$20</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="108" stopIfTrue="1">
+      <formula>B2=$X$21</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="109" stopIfTrue="1">
+      <formula>B2=$X$22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="110" stopIfTrue="1">
+      <formula>B2=$X$23</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="111" stopIfTrue="1">
+      <formula>B2=$X$24</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="112" stopIfTrue="1">
+      <formula>B2=$X$25</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="113" stopIfTrue="1">
+      <formula>B2=$X$26</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="114" stopIfTrue="1">
+      <formula>B2=$X$27</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="115" stopIfTrue="1">
+      <formula>B2=$X$28</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="116" stopIfTrue="1">
+      <formula>B2=$X$29</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="117" stopIfTrue="1">
+      <formula>B2=$X$30</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="118" stopIfTrue="1">
+      <formula>B2=$X$31</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="119" stopIfTrue="1">
+      <formula>B2=$X$32</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="120" stopIfTrue="1">
+      <formula>B2=$X$33</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="121" stopIfTrue="1">
+      <formula>B2=$X$34</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="122" stopIfTrue="1">
+      <formula>B2=$X$35</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="123" stopIfTrue="1">
+      <formula>B2=$X$36</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="124" stopIfTrue="1">
+      <formula>B2=$X$37</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="125" stopIfTrue="1">
+      <formula>B2=$X$38</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="126" stopIfTrue="1">
+      <formula>B2=$X$39</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="127" stopIfTrue="1">
+      <formula>B2=$X$40</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="128" stopIfTrue="1">
+      <formula>B2=$X$41</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="86" stopIfTrue="1">
+      <formula>B2=$Z$42</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:U25">
+    <cfRule type="expression" dxfId="42" priority="129">
+      <formula>ISBLANK(G2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="130" stopIfTrue="1">
+      <formula>"isblank(B2)"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="131" stopIfTrue="1">
+      <formula>G2=$X$2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="132" stopIfTrue="1">
+      <formula>G2=$X$3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="133" stopIfTrue="1">
+      <formula>G2=$X$4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="134" stopIfTrue="1">
+      <formula>G2=$X$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="135" stopIfTrue="1">
+      <formula>G2=$X$6</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="136" stopIfTrue="1">
+      <formula>G2=$X$7</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="137" stopIfTrue="1">
+      <formula>G2=$X$8</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="138" stopIfTrue="1">
+      <formula>G2=$X$9</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="139" stopIfTrue="1">
+      <formula>G2=$X$10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="140" stopIfTrue="1">
+      <formula>G2=$X$11</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="141" stopIfTrue="1">
+      <formula>G2=$X$12</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="142" stopIfTrue="1">
+      <formula>G2=$X$13</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="143" stopIfTrue="1">
+      <formula>G2=$X$14</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="144" stopIfTrue="1">
+      <formula>G2=$X$15</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="145" stopIfTrue="1">
+      <formula>G2=$X$16</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="146" stopIfTrue="1">
+      <formula>G2=$X$17</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="147" stopIfTrue="1">
+      <formula>G2=$X$18</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="148" stopIfTrue="1">
+      <formula>G2=$X$19</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="149" stopIfTrue="1">
+      <formula>G2=$X$20</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="150" stopIfTrue="1">
+      <formula>G2=$X$21</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="151" stopIfTrue="1">
+      <formula>G2=$X$22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="152" stopIfTrue="1">
+      <formula>G2=$X$23</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="153" stopIfTrue="1">
+      <formula>G2=$X$24</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="154" stopIfTrue="1">
+      <formula>G2=$X$25</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="155" stopIfTrue="1">
+      <formula>G2=$X$26</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="156" stopIfTrue="1">
+      <formula>G2=$X$27</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="157" stopIfTrue="1">
+      <formula>G2=$X$28</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="158" stopIfTrue="1">
+      <formula>G2=$X$29</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="159" stopIfTrue="1">
+      <formula>G2=$X$30</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="160" stopIfTrue="1">
+      <formula>G2=$X$31</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="161" stopIfTrue="1">
+      <formula>G2=$X$32</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="162" stopIfTrue="1">
+      <formula>G2=$X$33</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="163" stopIfTrue="1">
+      <formula>G2=$X$34</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="164" stopIfTrue="1">
+      <formula>G2=$X$35</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="165" stopIfTrue="1">
+      <formula>G2=$X$36</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="166" stopIfTrue="1">
+      <formula>G2=$X$37</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="167" stopIfTrue="1">
+      <formula>G2=$X$38</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="168" stopIfTrue="1">
+      <formula>G2=$X$39</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="169" stopIfTrue="1">
+      <formula>G2=$X$40</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="170" stopIfTrue="1">
+      <formula>G2=$X$41</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="172" stopIfTrue="1">
+      <formula>G2=$X$42</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>